<commit_message>
Gestion arrosage. Nouvelles commandes telnet.
</commit_message>
<xml_diff>
--- a/Outils/Pompe.xlsx
+++ b/Outils/Pompe.xlsx
@@ -49,7 +49,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -98,7 +98,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -783,11 +783,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-688479664"/>
-        <c:axId val="-688481296"/>
+        <c:axId val="-2102357920"/>
+        <c:axId val="-2102359552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-688479664"/>
+        <c:axId val="-2102357920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -914,12 +914,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-688481296"/>
+        <c:crossAx val="-2102359552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-688481296"/>
+        <c:axId val="-2102359552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1046,7 +1046,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-688479664"/>
+        <c:crossAx val="-2102357920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2020,7 +2020,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>